<commit_message>
Work Experience working code
</commit_message>
<xml_diff>
--- a/slingshot/TestData/InputData.xlsx
+++ b/slingshot/TestData/InputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2940" windowWidth="15120" windowHeight="1500" tabRatio="871" firstSheet="24" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="2940" windowWidth="15120" windowHeight="1500" tabRatio="871" firstSheet="20" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="ManageUsersSortBy_Success" sheetId="58" r:id="rId1"/>
@@ -27,50 +27,51 @@
     <sheet name="RemoveSkill_Success" sheetId="69" r:id="rId18"/>
     <sheet name="UserProfilePicUpload_Success" sheetId="68" r:id="rId19"/>
     <sheet name="Skills_Success" sheetId="66" r:id="rId20"/>
-    <sheet name="WorkExperience_Success" sheetId="64" r:id="rId21"/>
-    <sheet name="UserBaisicInfo_Failure" sheetId="65" r:id="rId22"/>
-    <sheet name="WorkExperience_Failure" sheetId="63" r:id="rId23"/>
-    <sheet name="UserEduQualification_Failure" sheetId="47" r:id="rId24"/>
-    <sheet name="UserEduQualification_Success" sheetId="48" r:id="rId25"/>
-    <sheet name="AddAdmins_Success" sheetId="49" r:id="rId26"/>
-    <sheet name="PodMinMaxFilter_Success" sheetId="36" r:id="rId27"/>
-    <sheet name="PodLevelFilter_Success" sheetId="35" r:id="rId28"/>
-    <sheet name="PodIndustryFilter_Success" sheetId="34" r:id="rId29"/>
-    <sheet name="Login_Failure" sheetId="10" r:id="rId30"/>
-    <sheet name="Login_Success" sheetId="7" r:id="rId31"/>
-    <sheet name="Organization_Failure" sheetId="30" r:id="rId32"/>
-    <sheet name="Organisation_Reg_Failure" sheetId="8" r:id="rId33"/>
-    <sheet name="ChangePassword_Failure" sheetId="11" r:id="rId34"/>
-    <sheet name="LoginAsSubAdmin_Success" sheetId="62" r:id="rId35"/>
-    <sheet name="ChangePassword_Success" sheetId="12" r:id="rId36"/>
-    <sheet name="PodSearch_Success" sheetId="13" r:id="rId37"/>
-    <sheet name="LoginAsAdmin_Success" sheetId="14" r:id="rId38"/>
-    <sheet name="EditOrgProfileForm_Success" sheetId="24" r:id="rId39"/>
-    <sheet name="EditOrgProfileForm_Failure" sheetId="26" r:id="rId40"/>
-    <sheet name="OrganizationUpload_Success" sheetId="31" r:id="rId41"/>
-    <sheet name="PodIconUpload_Success" sheetId="60" r:id="rId42"/>
-    <sheet name="PodIconUpload_Failure" sheetId="61" r:id="rId43"/>
-    <sheet name="RemoveIndustry_Success" sheetId="28" r:id="rId44"/>
-    <sheet name="EditAboutOrg_Success" sheetId="29" r:id="rId45"/>
-    <sheet name="LatestNews_Success" sheetId="32" r:id="rId46"/>
-    <sheet name="IndividualRegister_Failure" sheetId="15" r:id="rId47"/>
-    <sheet name="ForgotPassword_Failure" sheetId="16" r:id="rId48"/>
-    <sheet name="ForgotPassword_Success" sheetId="17" r:id="rId49"/>
-    <sheet name="AddAdmin_Success" sheetId="18" r:id="rId50"/>
-    <sheet name="AddAdmin_Failure" sheetId="19" r:id="rId51"/>
-    <sheet name="LoginAsRemovedAdmin_Success" sheetId="20" r:id="rId52"/>
-    <sheet name="AddAnotherAdmin_Success" sheetId="21" r:id="rId53"/>
-    <sheet name="PodsToBuy_Success" sheetId="51" r:id="rId54"/>
-    <sheet name="NoOfUsers_Success" sheetId="50" r:id="rId55"/>
-    <sheet name="NoOfUsers_Failure" sheetId="52" r:id="rId56"/>
-    <sheet name="LoginAsSalesAdmin_Success" sheetId="53" r:id="rId57"/>
+    <sheet name="WorkExperienceAddMore_Success" sheetId="70" r:id="rId21"/>
+    <sheet name="WorkExperience_Success" sheetId="64" r:id="rId22"/>
+    <sheet name="UserBaisicInfo_Failure" sheetId="65" r:id="rId23"/>
+    <sheet name="WorkExperience_Failure" sheetId="63" r:id="rId24"/>
+    <sheet name="UserEduQualification_Failure" sheetId="47" r:id="rId25"/>
+    <sheet name="UserEduQualification_Success" sheetId="48" r:id="rId26"/>
+    <sheet name="AddAdmins_Success" sheetId="49" r:id="rId27"/>
+    <sheet name="PodMinMaxFilter_Success" sheetId="36" r:id="rId28"/>
+    <sheet name="PodLevelFilter_Success" sheetId="35" r:id="rId29"/>
+    <sheet name="PodIndustryFilter_Success" sheetId="34" r:id="rId30"/>
+    <sheet name="Login_Failure" sheetId="10" r:id="rId31"/>
+    <sheet name="Login_Success" sheetId="7" r:id="rId32"/>
+    <sheet name="Organization_Failure" sheetId="30" r:id="rId33"/>
+    <sheet name="Organisation_Reg_Failure" sheetId="8" r:id="rId34"/>
+    <sheet name="ChangePassword_Failure" sheetId="11" r:id="rId35"/>
+    <sheet name="LoginAsSubAdmin_Success" sheetId="62" r:id="rId36"/>
+    <sheet name="ChangePassword_Success" sheetId="12" r:id="rId37"/>
+    <sheet name="PodSearch_Success" sheetId="13" r:id="rId38"/>
+    <sheet name="LoginAsAdmin_Success" sheetId="14" r:id="rId39"/>
+    <sheet name="EditOrgProfileForm_Success" sheetId="24" r:id="rId40"/>
+    <sheet name="EditOrgProfileForm_Failure" sheetId="26" r:id="rId41"/>
+    <sheet name="OrganizationUpload_Success" sheetId="31" r:id="rId42"/>
+    <sheet name="PodIconUpload_Success" sheetId="60" r:id="rId43"/>
+    <sheet name="PodIconUpload_Failure" sheetId="61" r:id="rId44"/>
+    <sheet name="RemoveIndustry_Success" sheetId="28" r:id="rId45"/>
+    <sheet name="EditAboutOrg_Success" sheetId="29" r:id="rId46"/>
+    <sheet name="LatestNews_Success" sheetId="32" r:id="rId47"/>
+    <sheet name="IndividualRegister_Failure" sheetId="15" r:id="rId48"/>
+    <sheet name="ForgotPassword_Failure" sheetId="16" r:id="rId49"/>
+    <sheet name="ForgotPassword_Success" sheetId="17" r:id="rId50"/>
+    <sheet name="AddAdmin_Success" sheetId="18" r:id="rId51"/>
+    <sheet name="AddAdmin_Failure" sheetId="19" r:id="rId52"/>
+    <sheet name="LoginAsRemovedAdmin_Success" sheetId="20" r:id="rId53"/>
+    <sheet name="AddAnotherAdmin_Success" sheetId="21" r:id="rId54"/>
+    <sheet name="PodsToBuy_Success" sheetId="51" r:id="rId55"/>
+    <sheet name="NoOfUsers_Success" sheetId="50" r:id="rId56"/>
+    <sheet name="NoOfUsers_Failure" sheetId="52" r:id="rId57"/>
+    <sheet name="LoginAsSalesAdmin_Success" sheetId="53" r:id="rId58"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="464">
   <si>
     <t>Expected Messages</t>
   </si>
@@ -1288,9 +1289,6 @@
     <t>Oct</t>
   </si>
   <si>
-    <t>MYINDUSTRY</t>
-  </si>
-  <si>
     <t>Certificate Name</t>
   </si>
   <si>
@@ -1450,7 +1448,22 @@
     <t>Number,Myerererererrr</t>
   </si>
   <si>
-    <t>9738801548</t>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>Sakha Global</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>Cerner Pvt Ltd</t>
+  </si>
+  <si>
+    <t>Civil Engineer</t>
+  </si>
+  <si>
+    <t>Construction Industry</t>
   </si>
 </sst>
 </file>
@@ -9092,7 +9105,7 @@
         <v>168</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C1" s="51" t="s">
         <v>283</v>
@@ -9100,7 +9113,7 @@
     </row>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>225</v>
@@ -9137,7 +9150,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -9162,7 +9175,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B1" s="51" t="s">
         <v>283</v>
@@ -9170,10 +9183,10 @@
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -9248,7 +9261,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -9262,6 +9275,89 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>376</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>379</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -9309,13 +9405,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>405</v>
+        <v>463</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>386</v>
+        <v>462</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>404</v>
+        <v>459</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>387</v>
@@ -9327,7 +9423,11 @@
         <v>389</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>342</v>
+        <v>341</v>
+      </c>
+      <c r="H2" s="37"/>
+      <c r="I2" s="2" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -9336,7 +9436,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
@@ -9410,7 +9510,7 @@
       <c r="L2" s="60"/>
       <c r="M2" s="60"/>
       <c r="N2" s="30" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -9424,7 +9524,7 @@
         <v>296</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>297</v>
@@ -9465,7 +9565,7 @@
         <v>295</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>297</v>
@@ -9483,7 +9583,7 @@
         <v>26</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>302</v>
@@ -9492,7 +9592,7 @@
         <v>371</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -9524,7 +9624,7 @@
         <v>26</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>302</v>
@@ -9533,7 +9633,7 @@
         <v>371</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -9550,7 +9650,7 @@
         <v>296</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>298</v>
@@ -9565,7 +9665,7 @@
         <v>26</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>302</v>
@@ -9574,7 +9674,7 @@
         <v>371</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -9591,10 +9691,10 @@
         <v>296</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>431</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>432</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>299</v>
@@ -9606,7 +9706,7 @@
         <v>26</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>302</v>
@@ -9615,7 +9715,7 @@
         <v>371</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -9632,10 +9732,10 @@
         <v>296</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>298</v>
@@ -9647,7 +9747,7 @@
         <v>300</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>302</v>
@@ -9673,10 +9773,10 @@
         <v>296</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>298</v>
@@ -9688,7 +9788,7 @@
         <v>300</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>302</v>
@@ -9714,10 +9814,10 @@
         <v>296</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>298</v>
@@ -9729,10 +9829,10 @@
         <v>300</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>302</v>
@@ -9741,7 +9841,7 @@
         <v>371</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -9758,10 +9858,10 @@
         <v>296</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>298</v>
@@ -9773,19 +9873,19 @@
         <v>300</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K11" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>444</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>371</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -9802,10 +9902,10 @@
         <v>296</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>298</v>
@@ -9817,19 +9917,19 @@
         <v>300</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>448</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>371</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -9852,7 +9952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -10177,7 +10277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
@@ -10281,13 +10381,13 @@
     </row>
     <row r="2" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B2" s="57" t="s">
         <v>327</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D2" s="56" t="s">
         <v>325</v>
@@ -10296,10 +10396,10 @@
         <v>326</v>
       </c>
       <c r="F2" s="56" t="s">
+        <v>410</v>
+      </c>
+      <c r="G2" s="56" t="s">
         <v>411</v>
-      </c>
-      <c r="G2" s="56" t="s">
-        <v>412</v>
       </c>
       <c r="H2" s="57" t="s">
         <v>329</v>
@@ -10308,16 +10408,16 @@
         <v>330</v>
       </c>
       <c r="J2" s="56" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K2" s="56" t="s">
         <v>332</v>
       </c>
       <c r="L2" s="56" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="M2" s="57" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="N2" s="57" t="s">
         <v>334</v>
@@ -10329,7 +10429,7 @@
         <v>332</v>
       </c>
       <c r="Q2" s="56" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="R2" s="57" t="s">
         <v>338</v>
@@ -10344,7 +10444,7 @@
         <v>336</v>
       </c>
       <c r="V2" s="57" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -10353,11 +10453,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -10449,7 +10549,7 @@
         <v>326</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D2" s="56" t="s">
         <v>343</v>
@@ -10458,7 +10558,7 @@
         <v>327</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G2" s="56" t="s">
         <v>328</v>
@@ -10470,10 +10570,10 @@
         <v>330</v>
       </c>
       <c r="J2" s="56" t="s">
+        <v>451</v>
+      </c>
+      <c r="K2" s="56" t="s">
         <v>452</v>
-      </c>
-      <c r="K2" s="56" t="s">
-        <v>453</v>
       </c>
       <c r="L2" s="56" t="s">
         <v>333</v>
@@ -10485,10 +10585,10 @@
         <v>334</v>
       </c>
       <c r="O2" s="56" t="s">
+        <v>453</v>
+      </c>
+      <c r="P2" s="56" t="s">
         <v>454</v>
-      </c>
-      <c r="P2" s="56" t="s">
-        <v>455</v>
       </c>
       <c r="Q2" s="56" t="s">
         <v>337</v>
@@ -10500,10 +10600,10 @@
         <v>339</v>
       </c>
       <c r="T2" s="56" t="s">
+        <v>455</v>
+      </c>
+      <c r="U2" s="56" t="s">
         <v>456</v>
-      </c>
-      <c r="U2" s="56" t="s">
-        <v>457</v>
       </c>
       <c r="V2" s="56" t="s">
         <v>345</v>
@@ -10515,7 +10615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -10681,7 +10781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -10732,7 +10832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -10778,59 +10878,6 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>185</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="28" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -10880,6 +10927,59 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10947,12 +11047,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10976,10 +11076,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>22</v>
+        <v>375</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -10995,7 +11095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -11149,7 +11249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
@@ -12012,7 +12112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -12146,7 +12246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -12191,7 +12291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -12279,7 +12379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -12330,7 +12430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -12375,7 +12475,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="25" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>357</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -12495,47 +12635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="25" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="50" t="s">
-        <v>357</v>
-      </c>
-      <c r="D1" s="50" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
@@ -13022,7 +13122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13059,7 +13159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13094,7 +13194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13129,7 +13229,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13166,7 +13266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13203,7 +13303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13240,7 +13340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
@@ -14145,7 +14245,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -14236,73 +14336,6 @@
       </c>
       <c r="E7" s="12" t="s">
         <v>112</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.85546875" style="7"/>
-    <col min="2" max="2" width="14.140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="34" style="7" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -14358,6 +14391,73 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="7"/>
+    <col min="2" max="2" width="14.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="34" style="7" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0"/>
@@ -14453,7 +14553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -14934,7 +15034,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -14978,7 +15078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -15076,7 +15176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -15110,7 +15210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -15144,7 +15244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -15180,7 +15280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Automation on seven December
</commit_message>
<xml_diff>
--- a/slingshot/TestData/InputData.xlsx
+++ b/slingshot/TestData/InputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2940" windowWidth="15120" windowHeight="1500" tabRatio="871" firstSheet="20" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="2940" windowWidth="15120" windowHeight="1500" tabRatio="871" firstSheet="16" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="ManageUsersSortBy_Success" sheetId="58" r:id="rId1"/>
@@ -23,55 +23,60 @@
     <sheet name="AnotherAdminErrorMsg_Success" sheetId="45" r:id="rId14"/>
     <sheet name="PostJob_Failure" sheetId="40" r:id="rId15"/>
     <sheet name="PostJob_Success" sheetId="59" r:id="rId16"/>
-    <sheet name="Certificate_Success" sheetId="67" r:id="rId17"/>
-    <sheet name="RemoveSkill_Success" sheetId="69" r:id="rId18"/>
-    <sheet name="UserProfilePicUpload_Success" sheetId="68" r:id="rId19"/>
-    <sheet name="Skills_Success" sheetId="66" r:id="rId20"/>
-    <sheet name="WorkExperienceAddMore_Success" sheetId="70" r:id="rId21"/>
-    <sheet name="WorkExperience_Success" sheetId="64" r:id="rId22"/>
-    <sheet name="UserBaisicInfo_Failure" sheetId="65" r:id="rId23"/>
-    <sheet name="WorkExperience_Failure" sheetId="63" r:id="rId24"/>
-    <sheet name="UserEduQualification_Failure" sheetId="47" r:id="rId25"/>
-    <sheet name="UserEduQualification_Success" sheetId="48" r:id="rId26"/>
-    <sheet name="AddAdmins_Success" sheetId="49" r:id="rId27"/>
-    <sheet name="PodMinMaxFilter_Success" sheetId="36" r:id="rId28"/>
-    <sheet name="PodLevelFilter_Success" sheetId="35" r:id="rId29"/>
-    <sheet name="PodIndustryFilter_Success" sheetId="34" r:id="rId30"/>
-    <sheet name="Login_Failure" sheetId="10" r:id="rId31"/>
-    <sheet name="Login_Success" sheetId="7" r:id="rId32"/>
-    <sheet name="Organization_Failure" sheetId="30" r:id="rId33"/>
-    <sheet name="Organisation_Reg_Failure" sheetId="8" r:id="rId34"/>
-    <sheet name="ChangePassword_Failure" sheetId="11" r:id="rId35"/>
-    <sheet name="LoginAsSubAdmin_Success" sheetId="62" r:id="rId36"/>
-    <sheet name="ChangePassword_Success" sheetId="12" r:id="rId37"/>
-    <sheet name="PodSearch_Success" sheetId="13" r:id="rId38"/>
-    <sheet name="LoginAsAdmin_Success" sheetId="14" r:id="rId39"/>
-    <sheet name="EditOrgProfileForm_Success" sheetId="24" r:id="rId40"/>
-    <sheet name="EditOrgProfileForm_Failure" sheetId="26" r:id="rId41"/>
-    <sheet name="OrganizationUpload_Success" sheetId="31" r:id="rId42"/>
-    <sheet name="PodIconUpload_Success" sheetId="60" r:id="rId43"/>
-    <sheet name="PodIconUpload_Failure" sheetId="61" r:id="rId44"/>
-    <sheet name="RemoveIndustry_Success" sheetId="28" r:id="rId45"/>
-    <sheet name="EditAboutOrg_Success" sheetId="29" r:id="rId46"/>
-    <sheet name="LatestNews_Success" sheetId="32" r:id="rId47"/>
-    <sheet name="IndividualRegister_Failure" sheetId="15" r:id="rId48"/>
-    <sheet name="ForgotPassword_Failure" sheetId="16" r:id="rId49"/>
-    <sheet name="ForgotPassword_Success" sheetId="17" r:id="rId50"/>
-    <sheet name="AddAdmin_Success" sheetId="18" r:id="rId51"/>
-    <sheet name="AddAdmin_Failure" sheetId="19" r:id="rId52"/>
-    <sheet name="LoginAsRemovedAdmin_Success" sheetId="20" r:id="rId53"/>
-    <sheet name="AddAnotherAdmin_Success" sheetId="21" r:id="rId54"/>
-    <sheet name="PodsToBuy_Success" sheetId="51" r:id="rId55"/>
-    <sheet name="NoOfUsers_Success" sheetId="50" r:id="rId56"/>
-    <sheet name="NoOfUsers_Failure" sheetId="52" r:id="rId57"/>
-    <sheet name="LoginAsSalesAdmin_Success" sheetId="53" r:id="rId58"/>
+    <sheet name="CertificateAddMore_Success" sheetId="75" r:id="rId17"/>
+    <sheet name="CertificateDelete_Success" sheetId="74" r:id="rId18"/>
+    <sheet name="CertificateEdit_Success" sheetId="73" r:id="rId19"/>
+    <sheet name="Certificate_Success" sheetId="67" r:id="rId20"/>
+    <sheet name="RemoveSkill_Success" sheetId="69" r:id="rId21"/>
+    <sheet name="UserProfilePicUpload_Success" sheetId="68" r:id="rId22"/>
+    <sheet name="Skills_Success" sheetId="66" r:id="rId23"/>
+    <sheet name="DeleteWorkExperience_Success" sheetId="71" r:id="rId24"/>
+    <sheet name="EditWorkExperience_Success" sheetId="72" r:id="rId25"/>
+    <sheet name="WorkExperienceAddMore_Success" sheetId="70" r:id="rId26"/>
+    <sheet name="WorkExperience_Success" sheetId="64" r:id="rId27"/>
+    <sheet name="UserBaisicInfo_Failure" sheetId="65" r:id="rId28"/>
+    <sheet name="WorkExperience_Failure" sheetId="63" r:id="rId29"/>
+    <sheet name="UserEduQualification_Failure" sheetId="47" r:id="rId30"/>
+    <sheet name="UserEduQualification_Success" sheetId="48" r:id="rId31"/>
+    <sheet name="AddAdmins_Success" sheetId="49" r:id="rId32"/>
+    <sheet name="PodMinMaxFilter_Success" sheetId="36" r:id="rId33"/>
+    <sheet name="PodLevelFilter_Success" sheetId="35" r:id="rId34"/>
+    <sheet name="PodIndustryFilter_Success" sheetId="34" r:id="rId35"/>
+    <sheet name="Login_Failure" sheetId="10" r:id="rId36"/>
+    <sheet name="Login_Success" sheetId="7" r:id="rId37"/>
+    <sheet name="Organization_Failure" sheetId="30" r:id="rId38"/>
+    <sheet name="Organisation_Reg_Failure" sheetId="8" r:id="rId39"/>
+    <sheet name="ChangePassword_Failure" sheetId="11" r:id="rId40"/>
+    <sheet name="LoginAsSubAdmin_Success" sheetId="62" r:id="rId41"/>
+    <sheet name="ChangePassword_Success" sheetId="12" r:id="rId42"/>
+    <sheet name="PodSearch_Success" sheetId="13" r:id="rId43"/>
+    <sheet name="LoginAsAdmin_Success" sheetId="14" r:id="rId44"/>
+    <sheet name="EditOrgProfileForm_Success" sheetId="24" r:id="rId45"/>
+    <sheet name="EditOrgProfileForm_Failure" sheetId="26" r:id="rId46"/>
+    <sheet name="OrganizationUpload_Success" sheetId="31" r:id="rId47"/>
+    <sheet name="PodIconUpload_Success" sheetId="60" r:id="rId48"/>
+    <sheet name="PodIconUpload_Failure" sheetId="61" r:id="rId49"/>
+    <sheet name="RemoveIndustry_Success" sheetId="28" r:id="rId50"/>
+    <sheet name="EditAboutOrg_Success" sheetId="29" r:id="rId51"/>
+    <sheet name="LatestNews_Success" sheetId="32" r:id="rId52"/>
+    <sheet name="IndividualRegister_Failure" sheetId="15" r:id="rId53"/>
+    <sheet name="ForgotPassword_Failure" sheetId="16" r:id="rId54"/>
+    <sheet name="ForgotPassword_Success" sheetId="17" r:id="rId55"/>
+    <sheet name="AddAdmin_Success" sheetId="18" r:id="rId56"/>
+    <sheet name="AddAdmin_Failure" sheetId="19" r:id="rId57"/>
+    <sheet name="LoginAsRemovedAdmin_Success" sheetId="20" r:id="rId58"/>
+    <sheet name="AddAnotherAdmin_Success" sheetId="21" r:id="rId59"/>
+    <sheet name="PodsToBuy_Success" sheetId="51" r:id="rId60"/>
+    <sheet name="NoOfUsers_Success" sheetId="50" r:id="rId61"/>
+    <sheet name="NoOfUsers_Failure" sheetId="52" r:id="rId62"/>
+    <sheet name="LoginAsSalesAdmin_Success" sheetId="53" r:id="rId63"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="471">
   <si>
     <t>Expected Messages</t>
   </si>
@@ -1292,178 +1297,199 @@
     <t>Certificate Name</t>
   </si>
   <si>
+    <t xml:space="preserve">J.S.S College for Medical Science </t>
+  </si>
+  <si>
+    <t>89.94</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>1988</t>
+  </si>
+  <si>
+    <t>59.49</t>
+  </si>
+  <si>
+    <t>56.49</t>
+  </si>
+  <si>
+    <t>yearPassGreaterThanBornYear,yearLessThanXYear,yearStartLessThanXYear,startYearLessThanXiiDiploma,startYearLessThanUg</t>
+  </si>
+  <si>
+    <t>ProfileImage Location</t>
+  </si>
+  <si>
+    <t>profileUploadSuccess</t>
+  </si>
+  <si>
+    <t>\Files\ValidProfileImage\ProfileImage</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>fname_req,age_req,gender_req,dob_req,maritalstatus_req,addline1_req,city_req,pin_req,emailid_req,mobile_req</t>
+  </si>
+  <si>
+    <t>1993-12-22</t>
+  </si>
+  <si>
+    <t>1995-12-01</t>
+  </si>
+  <si>
+    <t>560010</t>
+  </si>
+  <si>
+    <t>gender_req</t>
+  </si>
+  <si>
+    <t>560011</t>
+  </si>
+  <si>
+    <t>dob_req</t>
+  </si>
+  <si>
+    <t>1993-02-19</t>
+  </si>
+  <si>
+    <t>560012</t>
+  </si>
+  <si>
+    <t>maritalstatus_req</t>
+  </si>
+  <si>
+    <t>1992-01-20</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>560013</t>
+  </si>
+  <si>
+    <t>addline1_req</t>
+  </si>
+  <si>
+    <t>1974-07-07</t>
+  </si>
+  <si>
+    <t>560014</t>
+  </si>
+  <si>
+    <t>1947-08-15</t>
+  </si>
+  <si>
+    <t>Rewari</t>
+  </si>
+  <si>
+    <t>1947-08-16</t>
+  </si>
+  <si>
+    <t>5689</t>
+  </si>
+  <si>
+    <t>invalid_pin</t>
+  </si>
+  <si>
+    <t>1947-08-17</t>
+  </si>
+  <si>
+    <t>568978</t>
+  </si>
+  <si>
+    <t>adiyadav99@gmail.com</t>
+  </si>
+  <si>
+    <t>emailid_exists</t>
+  </si>
+  <si>
+    <t>1947-08-18</t>
+  </si>
+  <si>
+    <t>568979</t>
+  </si>
+  <si>
+    <t>adiyada9@</t>
+  </si>
+  <si>
+    <t>invalid_emailid</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>Number,Myerererererrr</t>
+  </si>
+  <si>
+    <t>Sakha Global</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>Cerner Pvt Ltd</t>
+  </si>
+  <si>
+    <t>Civil Engineer</t>
+  </si>
+  <si>
+    <t>Construction Industry</t>
+  </si>
+  <si>
+    <t>8050738344</t>
+  </si>
+  <si>
+    <t>Welcome2@</t>
+  </si>
+  <si>
+    <t>Computer Arch</t>
+  </si>
+  <si>
+    <t>Software Test Engineer</t>
+  </si>
+  <si>
+    <t>Xoriant Pvt Ltd</t>
+  </si>
+  <si>
+    <t>My Resume</t>
+  </si>
+  <si>
+    <t>PodWorksCertifiedAgriculturalMachineryIndustryTutorials</t>
+  </si>
+  <si>
     <t>F:\KPAutomationCode\automation\KPPhaseTwo\slingshot\Files\ValidProfileImage\ProfileImage</t>
   </si>
   <si>
-    <t xml:space="preserve">J.S.S College for Medical Science </t>
-  </si>
-  <si>
-    <t>89.94</t>
-  </si>
-  <si>
-    <t>1990</t>
-  </si>
-  <si>
-    <t>1989</t>
-  </si>
-  <si>
-    <t>83</t>
-  </si>
-  <si>
-    <t>1988</t>
-  </si>
-  <si>
-    <t>59.49</t>
-  </si>
-  <si>
-    <t>56.49</t>
-  </si>
-  <si>
-    <t>yearPassGreaterThanBornYear,yearLessThanXYear,yearStartLessThanXYear,startYearLessThanXiiDiploma,startYearLessThanUg</t>
-  </si>
-  <si>
-    <t>ProfileImage Location</t>
-  </si>
-  <si>
-    <t>profileUploadSuccess</t>
-  </si>
-  <si>
-    <t>\Files\ValidProfileImage\ProfileImage</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>fname_req,age_req,gender_req,dob_req,maritalstatus_req,addline1_req,city_req,pin_req,emailid_req,mobile_req</t>
-  </si>
-  <si>
-    <t>1993-12-22</t>
-  </si>
-  <si>
-    <t>1995-12-01</t>
-  </si>
-  <si>
-    <t>560010</t>
-  </si>
-  <si>
-    <t>gender_req</t>
-  </si>
-  <si>
-    <t>560011</t>
-  </si>
-  <si>
-    <t>dob_req</t>
-  </si>
-  <si>
-    <t>1993-02-19</t>
-  </si>
-  <si>
-    <t>560012</t>
-  </si>
-  <si>
-    <t>maritalstatus_req</t>
-  </si>
-  <si>
-    <t>1992-01-20</t>
-  </si>
-  <si>
-    <t>Married</t>
-  </si>
-  <si>
-    <t>560013</t>
-  </si>
-  <si>
-    <t>addline1_req</t>
-  </si>
-  <si>
-    <t>1974-07-07</t>
-  </si>
-  <si>
-    <t>560014</t>
-  </si>
-  <si>
-    <t>1947-08-15</t>
-  </si>
-  <si>
-    <t>Rewari</t>
-  </si>
-  <si>
-    <t>1947-08-16</t>
-  </si>
-  <si>
-    <t>5689</t>
-  </si>
-  <si>
-    <t>invalid_pin</t>
-  </si>
-  <si>
-    <t>1947-08-17</t>
-  </si>
-  <si>
-    <t>568978</t>
-  </si>
-  <si>
-    <t>adiyadav99@gmail.com</t>
-  </si>
-  <si>
-    <t>emailid_exists</t>
-  </si>
-  <si>
-    <t>1947-08-18</t>
-  </si>
-  <si>
-    <t>568979</t>
-  </si>
-  <si>
-    <t>adiyada9@</t>
-  </si>
-  <si>
-    <t>invalid_emailid</t>
-  </si>
-  <si>
-    <t>2001</t>
-  </si>
-  <si>
-    <t>2002</t>
-  </si>
-  <si>
-    <t>2003</t>
-  </si>
-  <si>
-    <t>2004</t>
-  </si>
-  <si>
-    <t>2005</t>
-  </si>
-  <si>
-    <t>2006</t>
-  </si>
-  <si>
-    <t>2007</t>
-  </si>
-  <si>
-    <t>2008</t>
-  </si>
-  <si>
-    <t>Number,Myerererererrr</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>Sakha Global</t>
-  </si>
-  <si>
-    <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>Cerner Pvt Ltd</t>
-  </si>
-  <si>
-    <t>Civil Engineer</t>
-  </si>
-  <si>
-    <t>Construction Industry</t>
+    <t>F:\KPAutomationCode\automation\KPPhaseTwo\slingshot\Files\ValidProfileImage\NewCertificate</t>
   </si>
 </sst>
 </file>
@@ -9088,15 +9114,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="46.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="2" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -9111,17 +9137,19 @@
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>406</v>
+        <v>470</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>225</v>
+        <v>468</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9130,27 +9158,27 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1:Y130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="B1" s="51" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>419</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -9163,30 +9191,30 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:K14"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="2" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="B1" s="51" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>418</v>
+    <row r="2" spans="1:2" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>467</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>417</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -9238,6 +9266,120 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>469</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>415</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9261,7 +9403,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -9270,12 +9412,131 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>376</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A3" sqref="A3:P52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="18.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>376</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>379</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>336</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9326,10 +9587,10 @@
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>387</v>
@@ -9353,12 +9614,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9405,13 +9666,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>387</v>
@@ -9419,13 +9680,9 @@
       <c r="E2" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>341</v>
-      </c>
-      <c r="H2" s="37"/>
+      <c r="H2" s="37" t="s">
+        <v>78</v>
+      </c>
       <c r="I2" s="2" t="s">
         <v>345</v>
       </c>
@@ -9436,7 +9693,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
@@ -9510,7 +9767,7 @@
       <c r="L2" s="60"/>
       <c r="M2" s="60"/>
       <c r="N2" s="30" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -9524,7 +9781,7 @@
         <v>296</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>297</v>
@@ -9565,7 +9822,7 @@
         <v>295</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>297</v>
@@ -9583,7 +9840,7 @@
         <v>26</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>302</v>
@@ -9592,7 +9849,7 @@
         <v>371</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -9624,7 +9881,7 @@
         <v>26</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>302</v>
@@ -9633,7 +9890,7 @@
         <v>371</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -9650,7 +9907,7 @@
         <v>296</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>298</v>
@@ -9665,7 +9922,7 @@
         <v>26</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>302</v>
@@ -9674,7 +9931,7 @@
         <v>371</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -9691,10 +9948,10 @@
         <v>296</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>431</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>299</v>
@@ -9706,7 +9963,7 @@
         <v>26</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>302</v>
@@ -9715,7 +9972,7 @@
         <v>371</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -9732,10 +9989,10 @@
         <v>296</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>298</v>
@@ -9747,7 +10004,7 @@
         <v>300</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>302</v>
@@ -9773,10 +10030,10 @@
         <v>296</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>298</v>
@@ -9788,7 +10045,7 @@
         <v>300</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>302</v>
@@ -9814,10 +10071,10 @@
         <v>296</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>298</v>
@@ -9829,10 +10086,10 @@
         <v>300</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>302</v>
@@ -9841,7 +10098,7 @@
         <v>371</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -9858,10 +10115,10 @@
         <v>296</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>298</v>
@@ -9873,19 +10130,19 @@
         <v>300</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K11" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>371</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -9902,10 +10159,10 @@
         <v>296</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>298</v>
@@ -9917,19 +10174,19 @@
         <v>300</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>446</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>447</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>371</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -9952,12 +10209,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10005,6 +10262,9 @@
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="I2" s="30" t="s">
         <v>384</v>
       </c>
@@ -10277,7 +10537,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="25" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>357</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
@@ -10381,13 +10681,13 @@
     </row>
     <row r="2" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B2" s="57" t="s">
         <v>327</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D2" s="56" t="s">
         <v>325</v>
@@ -10396,10 +10696,10 @@
         <v>326</v>
       </c>
       <c r="F2" s="56" t="s">
+        <v>409</v>
+      </c>
+      <c r="G2" s="56" t="s">
         <v>410</v>
-      </c>
-      <c r="G2" s="56" t="s">
-        <v>411</v>
       </c>
       <c r="H2" s="57" t="s">
         <v>329</v>
@@ -10408,16 +10708,16 @@
         <v>330</v>
       </c>
       <c r="J2" s="56" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K2" s="56" t="s">
         <v>332</v>
       </c>
       <c r="L2" s="56" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="M2" s="57" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="N2" s="57" t="s">
         <v>334</v>
@@ -10429,7 +10729,7 @@
         <v>332</v>
       </c>
       <c r="Q2" s="56" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="R2" s="57" t="s">
         <v>338</v>
@@ -10444,7 +10744,7 @@
         <v>336</v>
       </c>
       <c r="V2" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -10453,7 +10753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
@@ -10549,7 +10849,7 @@
         <v>326</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D2" s="56" t="s">
         <v>343</v>
@@ -10558,7 +10858,7 @@
         <v>327</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G2" s="56" t="s">
         <v>328</v>
@@ -10570,10 +10870,10 @@
         <v>330</v>
       </c>
       <c r="J2" s="56" t="s">
+        <v>450</v>
+      </c>
+      <c r="K2" s="56" t="s">
         <v>451</v>
-      </c>
-      <c r="K2" s="56" t="s">
-        <v>452</v>
       </c>
       <c r="L2" s="56" t="s">
         <v>333</v>
@@ -10585,10 +10885,10 @@
         <v>334</v>
       </c>
       <c r="O2" s="56" t="s">
+        <v>452</v>
+      </c>
+      <c r="P2" s="56" t="s">
         <v>453</v>
-      </c>
-      <c r="P2" s="56" t="s">
-        <v>454</v>
       </c>
       <c r="Q2" s="56" t="s">
         <v>337</v>
@@ -10600,10 +10900,10 @@
         <v>339</v>
       </c>
       <c r="T2" s="56" t="s">
+        <v>454</v>
+      </c>
+      <c r="U2" s="56" t="s">
         <v>455</v>
-      </c>
-      <c r="U2" s="56" t="s">
-        <v>456</v>
       </c>
       <c r="V2" s="56" t="s">
         <v>345</v>
@@ -10615,7 +10915,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -10781,7 +11081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -10832,7 +11132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -10885,47 +11185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="25" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="50" t="s">
-        <v>357</v>
-      </c>
-      <c r="D1" s="50" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -10978,7 +11238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -11047,7 +11307,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -11076,10 +11336,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>375</v>
+        <v>463</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -11095,7 +11355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -11249,7 +11509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
@@ -12112,7 +12372,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="25" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>357</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -12246,7 +12546,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -12291,7 +12591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -12379,7 +12679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -12430,7 +12730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -12475,47 +12775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="25" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="50" t="s">
-        <v>357</v>
-      </c>
-      <c r="D1" s="50" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -12635,7 +12895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
@@ -13122,7 +13382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13159,7 +13419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13194,7 +13454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13229,7 +13489,52 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13266,7 +13571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13303,7 +13608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13340,7 +13645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
@@ -14245,7 +14550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -14344,52 +14649,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -14456,7 +14716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK2"/>
   <sheetViews>
@@ -14553,7 +14813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -15034,7 +15294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -15078,7 +15338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -15173,150 +15433,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
-        <v>346</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
-        <v>351</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
-        <v>348</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
-        <v>348</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>352</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>353</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>355</v>
-      </c>
-      <c r="B2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -15373,6 +15489,150 @@
       <c r="A3" s="30"/>
       <c r="F3" s="30" t="s">
         <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>346</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="48" t="s">
+        <v>351</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>352</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>355</v>
+      </c>
+      <c r="B2" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>